<commit_message>
removed hardcodig for urls
</commit_message>
<xml_diff>
--- a/TestData_usgbc.xlsx
+++ b/TestData_usgbc.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="1440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16065" windowHeight="6465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
-    <sheet name="signin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="payment" sheetId="3" r:id="rId4"/>
+    <sheet name="URL" sheetId="5" r:id="rId2"/>
+    <sheet name="signin" sheetId="2" r:id="rId3"/>
+    <sheet name="contact" sheetId="4" r:id="rId4"/>
+    <sheet name="payment" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M19"/>
+  <oleSize ref="A1:L19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>firstname</t>
   </si>
@@ -227,6 +228,15 @@
   </si>
   <si>
     <t>sinha</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>https://test-dynamic-usgbc.pantheonsite.io</t>
+  </si>
+  <si>
+    <t>https://dev-dynamic-usgbc.pantheonsite.io</t>
   </si>
 </sst>
 </file>
@@ -591,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -791,6 +801,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -907,12 +954,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>

</xml_diff>

<commit_message>
values form testing file and browser setup to chrome
</commit_message>
<xml_diff>
--- a/TestData_usgbc.xlsx
+++ b/TestData_usgbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6465" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11340" windowHeight="3465" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="payment" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L19"/>
+  <oleSize ref="A1:G9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1037,7 +1037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
15-11-2017 added three test in comm Reg for there dues payment comparision with comm Reg page and payment page
</commit_message>
<xml_diff>
--- a/TestData_usgbc.xlsx
+++ b/TestData_usgbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="5865" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="5865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="payment" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
+  <oleSize ref="A1:N17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -841,7 +841,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
16-11-2017 modified all testcase failing coz of element not found exception
</commit_message>
<xml_diff>
--- a/TestData_usgbc.xlsx
+++ b/TestData_usgbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16485" windowHeight="5865" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13575" windowHeight="5865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>firstname</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>https://dev-dynamic-usgbc.pantheonsite.io</t>
+  </si>
+  <si>
+    <t>user doesnot exist</t>
+  </si>
+  <si>
+    <t>user which can do the payment for store with other user I get user not found</t>
   </si>
 </sst>
 </file>
@@ -841,12 +847,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,6 +919,9 @@
       <c r="B8" t="s">
         <v>57</v>
       </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -920,6 +930,9 @@
       <c r="B9" t="s">
         <v>66</v>
       </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -927,6 +940,9 @@
       </c>
       <c r="B10" t="s">
         <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new test script in donation for checking all the data is same in payment and receiopt page
</commit_message>
<xml_diff>
--- a/TestData_usgbc.xlsx
+++ b/TestData_usgbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5865" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15855" windowHeight="5865" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="payment" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P17"/>
+  <oleSize ref="A1:L17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
   <si>
     <t>firstname</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>Donation</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>$50</t>
+  </si>
+  <si>
+    <t>$100</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1202,7 +1211,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,8 +1241,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>25</v>
+      <c r="A2" t="s">
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
@@ -1249,8 +1258,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100</v>
+      <c r="A3" t="s">
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>100</v>
@@ -1266,8 +1275,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>150</v>
+      <c r="A4" t="s">
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>101</v>

</xml_diff>